<commit_message>
Mise à jour du mapping de l'entete (#78)
* MAJ du mapping de l'entete

* Mise à jour mapping entete c6acceb84ed590ac04ccf6a5afe7797876414dad
</commit_message>
<xml_diff>
--- a/main/ig/mappingPatientCDAFHIR.xlsx
+++ b/main/ig/mappingPatientCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="129">
   <si>
     <t>Property</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-10T16:53:25+00:00</t>
+    <t>2025-12-15T10:12:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -156,7 +156,7 @@
     <t>FRLMPatientUsager.personnePhysique.nomsPrenomsPatient.nom.nomNaissance</t>
   </si>
   <si>
-    <t>PrecordTarget.patientRole.patient.name.family@qualifier='BR'</t>
+    <t>recordTarget.patientRole.patient.name.family@qualifier='BR'</t>
   </si>
   <si>
     <t>FRLMPatientUsager.personnePhysique.nomsPrenomsPatient.nom.nomUtilise</t>
@@ -322,9 +322,6 @@
   </si>
   <si>
     <t>Patient.name.family</t>
-  </si>
-  <si>
-    <t>recordTarget.patientRole.patient.name.family@qualifier='BR'</t>
   </si>
   <si>
     <t>Patient.name:officialname.family</t>
@@ -1234,14 +1231,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1254,7 +1251,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1267,7 +1264,7 @@
         <v>33</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1280,7 +1277,7 @@
         <v>33</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1293,7 +1290,7 @@
         <v>33</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1306,7 +1303,7 @@
         <v>33</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -1319,7 +1316,7 @@
         <v>33</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1332,7 +1329,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -1345,7 +1342,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2"/>
     </row>
@@ -1358,7 +1355,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -1371,7 +1368,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="2"/>
     </row>
@@ -1384,7 +1381,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -1397,7 +1394,7 @@
         <v>33</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1410,7 +1407,7 @@
         <v>33</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -1423,7 +1420,7 @@
         <v>33</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -1436,7 +1433,7 @@
         <v>33</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -1449,7 +1446,7 @@
         <v>33</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -1462,7 +1459,7 @@
         <v>33</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -1475,7 +1472,7 @@
         <v>33</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1488,7 +1485,7 @@
         <v>33</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E28" s="2"/>
     </row>
@@ -1501,7 +1498,7 @@
         <v>33</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -1514,20 +1511,20 @@
         <v>33</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E31" s="2"/>
     </row>
@@ -1540,20 +1537,20 @@
         <v>33</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" s="2"/>
     </row>

</xml_diff>